<commit_message>
correct calobration and popup added when speed is out of calibration
</commit_message>
<xml_diff>
--- a/vitesse tapis vérification(2).xlsx
+++ b/vitesse tapis vérification(2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jparent1\Documents\GitHub\ISSUL-LeMur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AA2602-E7B4-43CD-9EB4-F74A50E971EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38C464A-F9D8-4A01-B9CC-5A04795F9BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="225" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="2" xr2:uid="{FB0E4987-4AAE-B84A-AAE7-9D6498FBF5E2}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="1" xr2:uid="{FB0E4987-4AAE-B84A-AAE7-9D6498FBF5E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="52">
   <si>
     <t xml:space="preserve">Angles </t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>tours</t>
+  </si>
+  <si>
+    <t>Pente</t>
+  </si>
+  <si>
+    <t>Vitesse asc</t>
   </si>
 </sst>
 </file>
@@ -234,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -445,11 +451,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -509,29 +526,47 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,15 +919,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -909,30 +944,30 @@
       <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="M2" s="37" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="M2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="38"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1076,17 +1111,17 @@
       <c r="J9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="38"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="38"/>
+      <c r="O9" s="33"/>
       <c r="P9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1306,12 +1341,12 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1339,19 +1374,19 @@
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="40"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1435,9 +1470,9 @@
       </c>
       <c r="L24" s="35"/>
       <c r="M24" s="35"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
@@ -1447,15 +1482,15 @@
       <c r="J25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K25" s="38" t="s">
+      <c r="K25" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="L25" s="38"/>
+      <c r="L25" s="33"/>
       <c r="M25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
       <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1620,12 +1655,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:C20"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="K24:M24"/>
@@ -1641,6 +1670,12 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I2:K2"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1648,847 +1683,994 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C2EF71-B620-4C63-A8E3-630AC35E5C32}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="2" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>37</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2.5030000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K3" s="9" t="s">
+    <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27" t="s">
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="E4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="28"/>
       <c r="F4" s="28"/>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="I4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="J4" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="K4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="11">
+      <c r="L4" s="11">
         <v>5.52</v>
       </c>
-      <c r="L4" s="12">
-        <f>K4*10</f>
+      <c r="M4" s="12">
+        <f>L4*10</f>
         <v>55.199999999999996</v>
       </c>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>18</v>
+      </c>
+      <c r="B5" s="40">
+        <v>600</v>
+      </c>
+      <c r="C5" s="44">
+        <v>80</v>
+      </c>
+      <c r="D5" s="44">
+        <v>50</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45">
+        <v>1.94</v>
+      </c>
+      <c r="H5" s="7">
+        <v>6.08</v>
+      </c>
+      <c r="I5" s="46">
+        <f>A5</f>
+        <v>18</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" ref="J5:J6" si="0">($M$4/C5)*3.6</f>
+        <v>2.484</v>
+      </c>
+      <c r="K5" s="21">
+        <f t="shared" ref="K5:K6" si="1">D5</f>
+        <v>50</v>
+      </c>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>18</v>
+      </c>
+      <c r="B6" s="40">
+        <v>600</v>
+      </c>
+      <c r="C6" s="44">
+        <v>80</v>
+      </c>
+      <c r="D6" s="44">
+        <v>80</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45">
+        <v>1.94</v>
+      </c>
+      <c r="H6" s="7">
+        <v>6.08</v>
+      </c>
+      <c r="I6" s="46">
+        <f>A6</f>
+        <v>18</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.484</v>
+      </c>
+      <c r="K6" s="21">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>18</v>
+      </c>
+      <c r="B7" s="40">
+        <v>800</v>
+      </c>
+      <c r="C7" s="6">
+        <v>75.73</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="G7" s="6">
+        <v>2.5880000000000001</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" ref="H5:H24" si="2">G7*$M$2</f>
+        <v>6.4777640000000005</v>
+      </c>
+      <c r="I7" s="46">
+        <f t="shared" ref="I7:I28" si="3">A7</f>
+        <v>18</v>
+      </c>
+      <c r="J7" s="7">
+        <f>($M$4/C7)*3.6</f>
+        <v>2.6240591575333418</v>
+      </c>
+      <c r="K7" s="21">
+        <f>D7</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>18</v>
+      </c>
+      <c r="B8" s="40">
+        <v>800</v>
+      </c>
+      <c r="C8" s="6">
+        <v>76.13</v>
+      </c>
+      <c r="D8" s="6">
+        <v>50</v>
+      </c>
+      <c r="E8" s="6">
+        <v>75.84</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2.5880000000000001</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="2"/>
+        <v>6.4777640000000005</v>
+      </c>
+      <c r="I8" s="46">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" ref="J8:J28" si="4">($M$4/C8)*3.6</f>
+        <v>2.6102719033232629</v>
+      </c>
+      <c r="K8" s="21">
+        <f t="shared" ref="K8:K28" si="5">D8</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="47">
+        <v>18</v>
+      </c>
+      <c r="B9" s="48">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7">
+        <v>3.2360000000000002</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="2"/>
+        <v>8.0997080000000015</v>
+      </c>
+      <c r="I9" s="46">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="4"/>
+        <v>3.3119999999999998</v>
+      </c>
+      <c r="K9" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="47">
         <v>22</v>
       </c>
-      <c r="B5" s="6">
-        <v>75.73</v>
-      </c>
-      <c r="C5">
-        <v>80</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2.5880000000000001</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" ref="G5:G22" si="0">F5*$L$2</f>
-        <v>6.4777640000000005</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" ref="H5:H18" si="1">LEFT(A5,3)</f>
-        <v xml:space="preserve">18 </v>
-      </c>
-      <c r="I5" s="7">
-        <f>($L$4/B5)*3.6</f>
-        <v>2.6240591575333418</v>
-      </c>
-      <c r="J5" s="21">
-        <f>C5</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B10" s="48">
+        <v>600</v>
+      </c>
+      <c r="C10">
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.601</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0073030000000003</v>
+      </c>
+      <c r="I10" s="46">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B6" s="6">
-        <v>76.13</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="J10" s="7">
+        <f t="shared" si="4"/>
+        <v>1.6288524590163933</v>
+      </c>
+      <c r="K10" s="21">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="D6" s="6">
-        <v>75.84</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6">
-        <v>2.5880000000000001</v>
-      </c>
-      <c r="G6" s="7">
-        <f t="shared" si="0"/>
-        <v>6.4777640000000005</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">18 </v>
-      </c>
-      <c r="I6" s="7">
-        <f t="shared" ref="I6:I26" si="2">($L$4/B6)*3.6</f>
-        <v>2.6102719033232629</v>
-      </c>
-      <c r="J6" s="21">
-        <f t="shared" ref="J6:J26" si="3">C6</f>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="47">
+        <v>22</v>
+      </c>
+      <c r="B11" s="48">
+        <v>600</v>
+      </c>
+      <c r="C11" s="7">
+        <v>120</v>
+      </c>
+      <c r="D11" s="7">
+        <v>80</v>
+      </c>
+      <c r="E11" s="7">
+        <v>124</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1.601</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0073030000000003</v>
+      </c>
+      <c r="I11" s="46">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="4"/>
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="K11" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="47">
+        <v>22</v>
+      </c>
+      <c r="B12" s="48">
+        <v>800</v>
+      </c>
+      <c r="C12" s="7">
+        <v>96</v>
+      </c>
+      <c r="D12" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7">
-        <v>60</v>
-      </c>
-      <c r="C7">
-        <v>80</v>
-      </c>
-      <c r="D7">
-        <v>60</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7">
-        <v>3.2360000000000002</v>
-      </c>
-      <c r="G7" s="7">
-        <f t="shared" si="0"/>
-        <v>8.0997080000000015</v>
-      </c>
-      <c r="H7" t="str">
-        <f>LEFT(A7,3)</f>
-        <v xml:space="preserve">18 </v>
-      </c>
-      <c r="I7" s="7">
-        <f t="shared" si="2"/>
-        <v>3.3119999999999998</v>
-      </c>
-      <c r="J7" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8">
-        <v>122</v>
-      </c>
-      <c r="C8">
+      <c r="E12" s="7"/>
+      <c r="G12" s="7">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="2"/>
+        <v>5.3439049999999995</v>
+      </c>
+      <c r="I12" s="46">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="4"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K12" s="21">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="F8" s="7">
-        <v>1.601</v>
-      </c>
-      <c r="G8" s="7">
-        <f t="shared" si="0"/>
-        <v>4.0073030000000003</v>
-      </c>
-      <c r="H8" t="str">
-        <f>LEFT(A8,3)</f>
-        <v xml:space="preserve">22 </v>
-      </c>
-      <c r="I8" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6288524590163933</v>
-      </c>
-      <c r="J8" s="21">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="47">
+        <v>22</v>
+      </c>
+      <c r="B13" s="48">
+        <v>800</v>
+      </c>
+      <c r="C13" s="7">
+        <v>90</v>
+      </c>
+      <c r="D13" s="7">
+        <v>80</v>
+      </c>
+      <c r="E13" s="7">
+        <v>92</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="2"/>
+        <v>5.3439049999999995</v>
+      </c>
+      <c r="I13" s="46">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="4"/>
+        <v>2.2079999999999997</v>
+      </c>
+      <c r="K13" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="47">
+        <v>22</v>
+      </c>
+      <c r="B14" s="48">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="7">
+        <v>74</v>
+      </c>
+      <c r="D14" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="7">
+      <c r="E14" s="7"/>
+      <c r="G14" s="7">
+        <v>2.669</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="2"/>
+        <v>6.6805070000000004</v>
+      </c>
+      <c r="I14" s="46">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="4"/>
+        <v>2.6854054054054051</v>
+      </c>
+      <c r="K14" s="21">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="47">
+        <v>22</v>
+      </c>
+      <c r="B15" s="48">
+        <v>1000</v>
+      </c>
+      <c r="C15">
+        <v>72</v>
+      </c>
+      <c r="D15">
+        <v>80</v>
+      </c>
+      <c r="E15">
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="7">
+        <v>2.669</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="2"/>
+        <v>6.6805070000000004</v>
+      </c>
+      <c r="I15" s="46">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="4"/>
+        <v>2.76</v>
+      </c>
+      <c r="K15" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="47">
+        <v>26</v>
+      </c>
+      <c r="B16" s="48">
+        <v>600</v>
+      </c>
+      <c r="C16" s="7">
+        <v>140</v>
+      </c>
+      <c r="D16" s="7">
+        <v>80</v>
+      </c>
+      <c r="E16" s="7">
+        <v>146</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1.3680000000000001</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="2"/>
+        <v>3.4241040000000003</v>
+      </c>
+      <c r="I16" s="46">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="4"/>
+        <v>1.4194285714285713</v>
+      </c>
+      <c r="K16" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>26</v>
+      </c>
+      <c r="B17" s="40">
+        <v>800</v>
+      </c>
+      <c r="C17" s="7">
+        <v>105</v>
+      </c>
+      <c r="D17" s="7">
+        <v>80</v>
+      </c>
+      <c r="E17" s="7">
+        <v>108</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17" s="7">
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="2"/>
+        <v>4.5654720000000006</v>
+      </c>
+      <c r="I17" s="46">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="4"/>
+        <v>1.8925714285714286</v>
+      </c>
+      <c r="K17" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>26</v>
+      </c>
+      <c r="B18" s="40">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="7">
+        <v>84</v>
+      </c>
+      <c r="D18" s="7">
+        <v>80</v>
+      </c>
+      <c r="E18" s="7">
+        <v>86</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="2"/>
+        <v>5.7093430000000005</v>
+      </c>
+      <c r="I18" s="46">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="4"/>
+        <v>2.3657142857142857</v>
+      </c>
+      <c r="K18" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>30</v>
+      </c>
+      <c r="B19" s="40">
+        <v>600</v>
+      </c>
+      <c r="C19" s="6">
+        <v>156</v>
+      </c>
+      <c r="D19" s="6">
+        <v>80</v>
+      </c>
+      <c r="E19" s="6">
+        <v>167</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="H19" s="7">
+        <f t="shared" si="2"/>
+        <v>3.0036</v>
+      </c>
+      <c r="I19" s="46">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="4"/>
+        <v>1.2738461538461539</v>
+      </c>
+      <c r="K19" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>30</v>
+      </c>
+      <c r="B20" s="40">
+        <v>800</v>
+      </c>
+      <c r="C20" s="6">
         <v>120</v>
       </c>
-      <c r="C9" s="7">
-        <v>80</v>
-      </c>
-      <c r="D9" s="7">
-        <v>124</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1.601</v>
-      </c>
-      <c r="G9" s="7">
-        <f t="shared" si="0"/>
-        <v>4.0073030000000003</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">22 </v>
-      </c>
-      <c r="I9" s="7">
-        <f t="shared" si="2"/>
+      <c r="D20" s="6">
+        <v>50</v>
+      </c>
+      <c r="E20" s="6">
+        <v>124.25</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0048000000000004</v>
+      </c>
+      <c r="I20" s="46">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="4"/>
         <v>1.6559999999999999</v>
       </c>
-      <c r="J9" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="K20" s="21">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>30</v>
+      </c>
+      <c r="B21" s="40">
+        <v>800</v>
+      </c>
+      <c r="C21" s="6">
+        <v>118.6</v>
+      </c>
+      <c r="D21" s="6">
+        <v>80</v>
+      </c>
+      <c r="E21" s="6">
+        <v>124.25</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0048000000000004</v>
+      </c>
+      <c r="I21" s="46">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="4"/>
+        <v>1.6755480607082631</v>
+      </c>
+      <c r="K21" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>30</v>
+      </c>
+      <c r="B22" s="40">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="7">
         <v>96</v>
       </c>
-      <c r="C10" s="7">
-        <v>50</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="F10" s="7">
-        <v>2.1349999999999998</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="0"/>
-        <v>5.3439049999999995</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">22 </v>
-      </c>
-      <c r="I10" s="7">
-        <f t="shared" si="2"/>
+      <c r="D22" s="6">
+        <v>80</v>
+      </c>
+      <c r="E22" s="7">
+        <v>98</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="2"/>
+        <v>5.0060000000000002</v>
+      </c>
+      <c r="I22" s="46">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="4"/>
         <v>2.0699999999999998</v>
       </c>
-      <c r="J10" s="21">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="7">
-        <v>90</v>
-      </c>
-      <c r="C11" s="7">
-        <v>80</v>
-      </c>
-      <c r="D11" s="7">
-        <v>92</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7">
-        <v>2.1349999999999998</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>5.3439049999999995</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">22 </v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" si="2"/>
-        <v>2.2079999999999997</v>
-      </c>
-      <c r="J11" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="7">
-        <v>74</v>
-      </c>
-      <c r="C12" s="7">
-        <v>50</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">22 </v>
-      </c>
-      <c r="I12" s="7">
-        <f t="shared" si="2"/>
-        <v>2.6854054054054051</v>
-      </c>
-      <c r="J12" s="21">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>72</v>
-      </c>
-      <c r="C13">
-        <v>80</v>
-      </c>
-      <c r="D13">
-        <v>74</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2.669</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>6.6805070000000004</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">22 </v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="2"/>
-        <v>2.76</v>
-      </c>
-      <c r="J13" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="7">
-        <v>140</v>
-      </c>
-      <c r="C14" s="7">
-        <v>80</v>
-      </c>
-      <c r="D14" s="7">
-        <v>146</v>
-      </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14" s="7">
-        <v>1.3680000000000001</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" si="0"/>
-        <v>3.4241040000000003</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">26 </v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4194285714285713</v>
-      </c>
-      <c r="J14" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="7">
-        <v>105</v>
-      </c>
-      <c r="C15" s="7">
-        <v>80</v>
-      </c>
-      <c r="D15" s="7">
-        <v>108</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15" s="7">
-        <v>1.8240000000000001</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="0"/>
-        <v>4.5654720000000006</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">26 </v>
-      </c>
-      <c r="I15" s="7">
-        <f t="shared" si="2"/>
-        <v>1.8925714285714286</v>
-      </c>
-      <c r="J15" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="7">
-        <v>84</v>
-      </c>
-      <c r="C16" s="7">
-        <v>80</v>
-      </c>
-      <c r="D16" s="7">
-        <v>86</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16" s="7">
-        <v>2.2810000000000001</v>
-      </c>
-      <c r="G16" s="7">
-        <f t="shared" si="0"/>
-        <v>5.7093430000000005</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">26 </v>
-      </c>
-      <c r="I16" s="7">
-        <f t="shared" si="2"/>
-        <v>2.3657142857142857</v>
-      </c>
-      <c r="J16" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="6">
-        <v>156</v>
-      </c>
-      <c r="C17" s="6">
-        <v>80</v>
-      </c>
-      <c r="D17" s="6">
-        <v>167</v>
-      </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="G17" s="7">
-        <f t="shared" si="0"/>
-        <v>3.0036</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">30 </v>
-      </c>
-      <c r="I17" s="7">
-        <f t="shared" si="2"/>
-        <v>1.2738461538461539</v>
-      </c>
-      <c r="J17" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6">
-        <v>120</v>
-      </c>
-      <c r="C18" s="6">
-        <v>50</v>
-      </c>
-      <c r="D18" s="6">
-        <v>124.25</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="G18" s="7">
-        <f t="shared" si="0"/>
-        <v>4.0048000000000004</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">30 </v>
-      </c>
-      <c r="I18" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6559999999999999</v>
-      </c>
-      <c r="J18" s="21">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="6">
-        <v>118.6</v>
-      </c>
-      <c r="C19" s="6">
-        <v>80</v>
-      </c>
-      <c r="D19" s="6">
-        <v>124.25</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="G19" s="7">
-        <f t="shared" si="0"/>
-        <v>4.0048000000000004</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" ref="H19:H26" si="4">LEFT(A19,3)</f>
-        <v xml:space="preserve">30 </v>
-      </c>
-      <c r="I19" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6755480607082631</v>
-      </c>
-      <c r="J19" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="7">
-        <v>96</v>
-      </c>
-      <c r="C20" s="6">
-        <v>80</v>
-      </c>
-      <c r="D20" s="7">
-        <v>98</v>
-      </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20" s="7">
-        <v>2</v>
-      </c>
-      <c r="G20" s="7">
-        <f t="shared" si="0"/>
-        <v>5.0060000000000002</v>
-      </c>
-      <c r="H20" t="str">
+      <c r="K22" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>38</v>
+      </c>
+      <c r="B23" s="40">
+        <v>600</v>
+      </c>
+      <c r="C23" s="7">
+        <v>186</v>
+      </c>
+      <c r="D23" s="7">
+        <v>80</v>
+      </c>
+      <c r="E23" s="7">
+        <v>208</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="2"/>
+        <v>2.4379219999999999</v>
+      </c>
+      <c r="I23" s="46">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="J23" s="7">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">30 </v>
-      </c>
-      <c r="I20" s="7">
-        <f t="shared" si="2"/>
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="J20" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="7">
-        <v>186</v>
-      </c>
-      <c r="C21" s="7">
-        <v>80</v>
-      </c>
-      <c r="D21" s="7">
-        <v>208</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="G21" s="7">
-        <f t="shared" si="0"/>
-        <v>2.4379219999999999</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">38 </v>
-      </c>
-      <c r="I21" s="7">
-        <f t="shared" si="2"/>
         <v>1.0683870967741935</v>
       </c>
-      <c r="J21" s="21">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="6">
+      <c r="K23" s="21">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>38</v>
+      </c>
+      <c r="B24" s="40">
+        <v>600</v>
+      </c>
+      <c r="C24" s="6">
         <f>96.46*2</f>
         <v>192.92</v>
       </c>
-      <c r="C22" s="6">
+      <c r="D24" s="6">
         <v>50</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="F22" s="7">
+      <c r="E24" s="6"/>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24" s="7">
         <v>0.97399999999999998</v>
       </c>
-      <c r="G22" s="7">
-        <f t="shared" si="0"/>
+      <c r="H24" s="7">
+        <f t="shared" si="2"/>
         <v>2.4379219999999999</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">38 </v>
-      </c>
-      <c r="I22" s="7">
-        <f>($L$4/B22)*3.6</f>
+      <c r="I24" s="46">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="J24" s="7">
+        <f>($M$4/C24)*3.6</f>
         <v>1.0300642753472942</v>
       </c>
-      <c r="J22" s="21">
-        <f>C22</f>
+      <c r="K24" s="21">
+        <f>D24</f>
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="6">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>38</v>
+      </c>
+      <c r="B25" s="40">
+        <v>800</v>
+      </c>
+      <c r="C25" s="6">
         <v>142.37</v>
       </c>
-      <c r="C23" s="6">
-        <v>80</v>
-      </c>
-      <c r="D23" s="6">
+      <c r="D25" s="6">
+        <v>80</v>
+      </c>
+      <c r="E25" s="6">
         <v>152.86000000000001</v>
       </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6">
         <v>1.2989999999999999</v>
       </c>
-      <c r="G23" s="7">
-        <f>F23*$L$2</f>
+      <c r="H25" s="7">
+        <f>G25*$M$2</f>
         <v>3.2513969999999999</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">38 </v>
-      </c>
-      <c r="I23" s="7">
-        <f>($L$4/B23)*3.6</f>
+      <c r="I25" s="46">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="J25" s="7">
+        <f>($M$4/C25)*3.6</f>
         <v>1.3957996768982228</v>
       </c>
-      <c r="J23" s="21">
-        <f>C23</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="6">
+      <c r="K25" s="21">
+        <f>D25</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>38</v>
+      </c>
+      <c r="B26" s="40">
+        <v>800</v>
+      </c>
+      <c r="C26" s="6">
         <v>146</v>
       </c>
-      <c r="C24" s="6">
+      <c r="D26" s="6">
         <v>50</v>
       </c>
-      <c r="D24" s="6">
+      <c r="E26" s="6">
         <v>152.86000000000001</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G26" s="6">
         <v>1.2989999999999999</v>
       </c>
-      <c r="G24" s="7">
-        <f>F24*$L$2</f>
+      <c r="H26" s="7">
+        <f>G26*$M$2</f>
         <v>3.2513969999999999</v>
       </c>
-      <c r="H24" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">38 </v>
-      </c>
-      <c r="I24" s="7">
-        <f>($L$4/B24)*3.6</f>
+      <c r="I26" s="46">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="J26" s="7">
+        <f>($M$4/C26)*3.6</f>
         <v>1.3610958904109587</v>
       </c>
-      <c r="J24" s="21">
-        <f>C24</f>
+      <c r="K26" s="21">
+        <f>D26</f>
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="6">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>38</v>
+      </c>
+      <c r="B27" s="40">
+        <v>1000</v>
+      </c>
+      <c r="C27" s="6">
         <f>59*2</f>
         <v>118</v>
       </c>
-      <c r="C25" s="6">
+      <c r="D27" s="6">
         <v>50</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25">
-        <v>10</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E27" s="6"/>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27" s="6">
         <v>1.62</v>
       </c>
-      <c r="G25" s="7">
-        <f>F25*$L$2</f>
+      <c r="H27" s="7">
+        <f>G27*$M$2</f>
         <v>4.0548600000000006</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I27" s="46">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="J27" s="7">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">38 </v>
-      </c>
-      <c r="I25" s="7">
-        <f t="shared" si="2"/>
         <v>1.6840677966101694</v>
       </c>
-      <c r="J25" s="21">
-        <f t="shared" si="3"/>
+      <c r="K27" s="21">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="22">
+    <row r="28" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>38</v>
+      </c>
+      <c r="B28" s="43">
+        <v>1000</v>
+      </c>
+      <c r="C28" s="22">
         <v>114</v>
       </c>
-      <c r="C26" s="22">
-        <v>80</v>
-      </c>
-      <c r="D26" s="22">
+      <c r="D28" s="22">
+        <v>80</v>
+      </c>
+      <c r="E28" s="22">
         <v>122</v>
       </c>
-      <c r="E26" s="23">
-        <v>10</v>
-      </c>
-      <c r="F26" s="24">
+      <c r="F28" s="23">
+        <v>10</v>
+      </c>
+      <c r="G28" s="24">
         <v>1.6240000000000001</v>
       </c>
-      <c r="G26" s="24">
-        <f>F26*$L$2</f>
+      <c r="H28" s="24">
+        <f>G28*$M$2</f>
         <v>4.0648720000000003</v>
       </c>
-      <c r="H26" s="23" t="str">
+      <c r="I28" s="46">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="J28" s="24">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">38 </v>
-      </c>
-      <c r="I26" s="24">
-        <f t="shared" si="2"/>
         <v>1.743157894736842</v>
       </c>
-      <c r="J26" s="25">
-        <f t="shared" si="3"/>
+      <c r="K28" s="25">
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2498,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F7122E-A639-469D-A85E-583921DE1214}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3926,7 +4108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94051208-C44B-408D-8037-3B9D5E83D8BC}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3936,11 +4118,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>

</xml_diff>

<commit_message>
improved lookup table generator
</commit_message>
<xml_diff>
--- a/vitesse tapis vérification(2).xlsx
+++ b/vitesse tapis vérification(2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jparent1\Documents\GitHub\ISSUL-LeMur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38C464A-F9D8-4A01-B9CC-5A04795F9BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E4F446-56E3-426D-AE63-3A563E699D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="1" xr2:uid="{FB0E4987-4AAE-B84A-AAE7-9D6498FBF5E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="4" xr2:uid="{FB0E4987-4AAE-B84A-AAE7-9D6498FBF5E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Mode escalier" sheetId="4" r:id="rId3"/>
     <sheet name="Mode escalier (2)" sheetId="6" r:id="rId4"/>
     <sheet name="Mode bande (2)" sheetId="7" r:id="rId5"/>
-    <sheet name="Feuil2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="52">
   <si>
     <t xml:space="preserve">Angles </t>
   </si>
@@ -466,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -499,9 +498,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,47 +522,32 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,15 +900,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -944,30 +925,30 @@
       <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="M2" s="36" t="s">
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="M2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1111,17 +1092,17 @@
       <c r="J9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="33"/>
+      <c r="L9" s="38"/>
       <c r="M9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="N9" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="33"/>
+      <c r="O9" s="38"/>
       <c r="P9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1341,12 +1322,12 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1374,19 +1355,19 @@
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1470,9 +1451,9 @@
       </c>
       <c r="L24" s="35"/>
       <c r="M24" s="35"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
@@ -1482,15 +1463,15 @@
       <c r="J25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="L25" s="33"/>
+      <c r="L25" s="38"/>
       <c r="M25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
       <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1655,6 +1636,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="K24:M24"/>
@@ -1670,12 +1657,6 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1685,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C2EF71-B620-4C63-A8E3-630AC35E5C32}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -1695,11 +1676,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2" s="6"/>
@@ -1728,33 +1709,33 @@
       <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="28" t="s">
         <v>44</v>
       </c>
       <c r="L4" s="11">
@@ -1770,24 +1751,23 @@
       <c r="A5" s="3">
         <v>18</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="29">
         <v>600</v>
       </c>
-      <c r="C5" s="44">
-        <v>80</v>
-      </c>
-      <c r="D5" s="44">
+      <c r="C5" s="6">
+        <v>80</v>
+      </c>
+      <c r="D5" s="6">
         <v>50</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45">
+      <c r="E5" s="6"/>
+      <c r="G5">
         <v>1.94</v>
       </c>
       <c r="H5" s="7">
         <v>6.08</v>
       </c>
-      <c r="I5" s="46">
+      <c r="I5" s="7">
         <f>A5</f>
         <v>18</v>
       </c>
@@ -1795,36 +1775,32 @@
         <f t="shared" ref="J5:J6" si="0">($M$4/C5)*3.6</f>
         <v>2.484</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="20">
         <f t="shared" ref="K5:K6" si="1">D5</f>
         <v>50</v>
       </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>18</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="29">
         <v>600</v>
       </c>
-      <c r="C6" s="44">
-        <v>80</v>
-      </c>
-      <c r="D6" s="44">
-        <v>80</v>
-      </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45">
+      <c r="C6" s="6">
+        <v>80</v>
+      </c>
+      <c r="D6" s="6">
+        <v>80</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="G6">
         <v>1.94</v>
       </c>
       <c r="H6" s="7">
         <v>6.08</v>
       </c>
-      <c r="I6" s="46">
+      <c r="I6" s="7">
         <f>A6</f>
         <v>18</v>
       </c>
@@ -1832,19 +1808,16 @@
         <f t="shared" si="0"/>
         <v>2.484</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="20">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>18</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="29">
         <v>800</v>
       </c>
       <c r="C7" s="6">
@@ -1857,10 +1830,10 @@
         <v>2.5880000000000001</v>
       </c>
       <c r="H7" s="7">
-        <f t="shared" ref="H5:H24" si="2">G7*$M$2</f>
+        <f t="shared" ref="H7:H24" si="2">G7*$M$2</f>
         <v>6.4777640000000005</v>
       </c>
-      <c r="I7" s="46">
+      <c r="I7" s="7">
         <f t="shared" ref="I7:I28" si="3">A7</f>
         <v>18</v>
       </c>
@@ -1868,7 +1841,7 @@
         <f>($M$4/C7)*3.6</f>
         <v>2.6240591575333418</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="20">
         <f>D7</f>
         <v>80</v>
       </c>
@@ -1877,7 +1850,7 @@
       <c r="A8" s="3">
         <v>18</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="29">
         <v>800</v>
       </c>
       <c r="C8" s="6">
@@ -1899,7 +1872,7 @@
         <f t="shared" si="2"/>
         <v>6.4777640000000005</v>
       </c>
-      <c r="I8" s="46">
+      <c r="I8" s="7">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -1907,16 +1880,16 @@
         <f t="shared" ref="J8:J28" si="4">($M$4/C8)*3.6</f>
         <v>2.6102719033232629</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="20">
         <f t="shared" ref="K8:K28" si="5">D8</f>
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="3">
         <v>18</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="29">
         <v>1000</v>
       </c>
       <c r="C9">
@@ -1938,7 +1911,7 @@
         <f t="shared" si="2"/>
         <v>8.0997080000000015</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="7">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -1946,16 +1919,16 @@
         <f t="shared" si="4"/>
         <v>3.3119999999999998</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="A10" s="3">
         <v>22</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="29">
         <v>600</v>
       </c>
       <c r="C10">
@@ -1971,7 +1944,7 @@
         <f t="shared" si="2"/>
         <v>4.0073030000000003</v>
       </c>
-      <c r="I10" s="46">
+      <c r="I10" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -1979,16 +1952,16 @@
         <f t="shared" si="4"/>
         <v>1.6288524590163933</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="20">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="47">
+      <c r="A11" s="3">
         <v>22</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="29">
         <v>600</v>
       </c>
       <c r="C11" s="7">
@@ -2010,7 +1983,7 @@
         <f t="shared" si="2"/>
         <v>4.0073030000000003</v>
       </c>
-      <c r="I11" s="46">
+      <c r="I11" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -2018,16 +1991,16 @@
         <f t="shared" si="4"/>
         <v>1.6559999999999999</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="3">
         <v>22</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="29">
         <v>800</v>
       </c>
       <c r="C12" s="7">
@@ -2044,7 +2017,7 @@
         <f t="shared" si="2"/>
         <v>5.3439049999999995</v>
       </c>
-      <c r="I12" s="46">
+      <c r="I12" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -2052,16 +2025,16 @@
         <f t="shared" si="4"/>
         <v>2.0699999999999998</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="20">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
+      <c r="A13" s="3">
         <v>22</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="29">
         <v>800</v>
       </c>
       <c r="C13" s="7">
@@ -2083,7 +2056,7 @@
         <f t="shared" si="2"/>
         <v>5.3439049999999995</v>
       </c>
-      <c r="I13" s="46">
+      <c r="I13" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -2091,16 +2064,16 @@
         <f t="shared" si="4"/>
         <v>2.2079999999999997</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="47">
+      <c r="A14" s="3">
         <v>22</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="29">
         <v>1000</v>
       </c>
       <c r="C14" s="7">
@@ -2117,7 +2090,7 @@
         <f t="shared" si="2"/>
         <v>6.6805070000000004</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -2125,16 +2098,16 @@
         <f t="shared" si="4"/>
         <v>2.6854054054054051</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="20">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="3">
         <v>22</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="29">
         <v>1000</v>
       </c>
       <c r="C15">
@@ -2156,7 +2129,7 @@
         <f t="shared" si="2"/>
         <v>6.6805070000000004</v>
       </c>
-      <c r="I15" s="46">
+      <c r="I15" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -2164,16 +2137,16 @@
         <f t="shared" si="4"/>
         <v>2.76</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="47">
+      <c r="A16" s="3">
         <v>26</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="29">
         <v>600</v>
       </c>
       <c r="C16" s="7">
@@ -2195,7 +2168,7 @@
         <f t="shared" si="2"/>
         <v>3.4241040000000003</v>
       </c>
-      <c r="I16" s="46">
+      <c r="I16" s="7">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -2203,7 +2176,7 @@
         <f t="shared" si="4"/>
         <v>1.4194285714285713</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2212,7 +2185,7 @@
       <c r="A17" s="3">
         <v>26</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="29">
         <v>800</v>
       </c>
       <c r="C17" s="7">
@@ -2234,7 +2207,7 @@
         <f t="shared" si="2"/>
         <v>4.5654720000000006</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="7">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -2242,7 +2215,7 @@
         <f t="shared" si="4"/>
         <v>1.8925714285714286</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2251,7 +2224,7 @@
       <c r="A18" s="3">
         <v>26</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="29">
         <v>1000</v>
       </c>
       <c r="C18" s="7">
@@ -2273,7 +2246,7 @@
         <f t="shared" si="2"/>
         <v>5.7093430000000005</v>
       </c>
-      <c r="I18" s="46">
+      <c r="I18" s="7">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -2281,7 +2254,7 @@
         <f t="shared" si="4"/>
         <v>2.3657142857142857</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2290,7 +2263,7 @@
       <c r="A19" s="3">
         <v>30</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="29">
         <v>600</v>
       </c>
       <c r="C19" s="6">
@@ -2312,7 +2285,7 @@
         <f t="shared" si="2"/>
         <v>3.0036</v>
       </c>
-      <c r="I19" s="46">
+      <c r="I19" s="7">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -2320,7 +2293,7 @@
         <f t="shared" si="4"/>
         <v>1.2738461538461539</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2329,7 +2302,7 @@
       <c r="A20" s="3">
         <v>30</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="29">
         <v>800</v>
       </c>
       <c r="C20" s="6">
@@ -2348,7 +2321,7 @@
         <f t="shared" si="2"/>
         <v>4.0048000000000004</v>
       </c>
-      <c r="I20" s="46">
+      <c r="I20" s="7">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -2356,7 +2329,7 @@
         <f t="shared" si="4"/>
         <v>1.6559999999999999</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="20">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
@@ -2365,7 +2338,7 @@
       <c r="A21" s="3">
         <v>30</v>
       </c>
-      <c r="B21" s="40">
+      <c r="B21" s="29">
         <v>800</v>
       </c>
       <c r="C21" s="6">
@@ -2387,7 +2360,7 @@
         <f t="shared" si="2"/>
         <v>4.0048000000000004</v>
       </c>
-      <c r="I21" s="46">
+      <c r="I21" s="7">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -2395,7 +2368,7 @@
         <f t="shared" si="4"/>
         <v>1.6755480607082631</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2404,7 +2377,7 @@
       <c r="A22" s="3">
         <v>30</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="29">
         <v>1000</v>
       </c>
       <c r="C22" s="7">
@@ -2426,7 +2399,7 @@
         <f t="shared" si="2"/>
         <v>5.0060000000000002</v>
       </c>
-      <c r="I22" s="46">
+      <c r="I22" s="7">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -2434,7 +2407,7 @@
         <f t="shared" si="4"/>
         <v>2.0699999999999998</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K22" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2443,7 +2416,7 @@
       <c r="A23" s="3">
         <v>38</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="29">
         <v>600</v>
       </c>
       <c r="C23" s="7">
@@ -2465,7 +2438,7 @@
         <f t="shared" si="2"/>
         <v>2.4379219999999999</v>
       </c>
-      <c r="I23" s="46">
+      <c r="I23" s="7">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -2473,7 +2446,7 @@
         <f t="shared" si="4"/>
         <v>1.0683870967741935</v>
       </c>
-      <c r="K23" s="21">
+      <c r="K23" s="20">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2482,7 +2455,7 @@
       <c r="A24" s="3">
         <v>38</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="29">
         <v>600</v>
       </c>
       <c r="C24" s="6">
@@ -2503,7 +2476,7 @@
         <f t="shared" si="2"/>
         <v>2.4379219999999999</v>
       </c>
-      <c r="I24" s="46">
+      <c r="I24" s="7">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -2511,7 +2484,7 @@
         <f>($M$4/C24)*3.6</f>
         <v>1.0300642753472942</v>
       </c>
-      <c r="K24" s="21">
+      <c r="K24" s="20">
         <f>D24</f>
         <v>50</v>
       </c>
@@ -2520,7 +2493,7 @@
       <c r="A25" s="3">
         <v>38</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="29">
         <v>800</v>
       </c>
       <c r="C25" s="6">
@@ -2542,7 +2515,7 @@
         <f>G25*$M$2</f>
         <v>3.2513969999999999</v>
       </c>
-      <c r="I25" s="46">
+      <c r="I25" s="7">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -2550,7 +2523,7 @@
         <f>($M$4/C25)*3.6</f>
         <v>1.3957996768982228</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="20">
         <f>D25</f>
         <v>80</v>
       </c>
@@ -2559,7 +2532,7 @@
       <c r="A26" s="3">
         <v>38</v>
       </c>
-      <c r="B26" s="40">
+      <c r="B26" s="29">
         <v>800</v>
       </c>
       <c r="C26" s="6">
@@ -2578,7 +2551,7 @@
         <f>G26*$M$2</f>
         <v>3.2513969999999999</v>
       </c>
-      <c r="I26" s="46">
+      <c r="I26" s="7">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -2586,7 +2559,7 @@
         <f>($M$4/C26)*3.6</f>
         <v>1.3610958904109587</v>
       </c>
-      <c r="K26" s="21">
+      <c r="K26" s="20">
         <f>D26</f>
         <v>50</v>
       </c>
@@ -2595,7 +2568,7 @@
       <c r="A27" s="3">
         <v>38</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="29">
         <v>1000</v>
       </c>
       <c r="C27" s="6">
@@ -2616,7 +2589,7 @@
         <f>G27*$M$2</f>
         <v>4.0548600000000006</v>
       </c>
-      <c r="I27" s="46">
+      <c r="I27" s="7">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -2624,7 +2597,7 @@
         <f t="shared" si="4"/>
         <v>1.6840677966101694</v>
       </c>
-      <c r="K27" s="21">
+      <c r="K27" s="20">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
@@ -2633,37 +2606,37 @@
       <c r="A28" s="3">
         <v>38</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="33">
         <v>1000</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="21">
         <v>114</v>
       </c>
-      <c r="D28" s="22">
-        <v>80</v>
-      </c>
-      <c r="E28" s="22">
+      <c r="D28" s="21">
+        <v>80</v>
+      </c>
+      <c r="E28" s="21">
         <v>122</v>
       </c>
-      <c r="F28" s="23">
-        <v>10</v>
-      </c>
-      <c r="G28" s="24">
+      <c r="F28" s="22">
+        <v>10</v>
+      </c>
+      <c r="G28" s="23">
         <v>1.6240000000000001</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="23">
         <f>G28*$M$2</f>
         <v>4.0648720000000003</v>
       </c>
-      <c r="I28" s="46">
+      <c r="I28" s="7">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J28" s="23">
         <f t="shared" si="4"/>
         <v>1.743157894736842</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="24">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
@@ -2851,7 +2824,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B6">
@@ -2921,7 +2894,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2">
@@ -2991,7 +2964,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="7">
@@ -3311,7 +3284,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="17">
@@ -3484,7 +3457,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B24">
@@ -3531,7 +3504,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3887,8 +3860,12 @@
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="4">
+        <v>124</v>
+      </c>
+      <c r="C13" s="18">
+        <v>74</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13">
         <v>10</v>
@@ -3904,13 +3881,13 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">30 </v>
       </c>
-      <c r="I13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>1.6316129032258067</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4108,8 +4085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94051208-C44B-408D-8037-3B9D5E83D8BC}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4118,11 +4095,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -4151,30 +4128,30 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>44</v>
       </c>
       <c r="K4" s="11">
@@ -4206,7 +4183,7 @@
         <f>($L$4/B5)*3.6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="20">
         <f>C5</f>
         <v>0</v>
       </c>
@@ -4236,7 +4213,7 @@
         <f t="shared" ref="I6:I22" si="2">($L$4/B6)*3.6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="20">
         <f t="shared" ref="J6:J22" si="3">C6</f>
         <v>0</v>
       </c>
@@ -4263,7 +4240,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4293,7 +4270,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4323,7 +4300,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4350,7 +4327,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4380,7 +4357,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4410,7 +4387,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4440,7 +4417,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4470,7 +4447,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4479,7 +4456,9 @@
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6">
+        <v>124</v>
+      </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="F15" s="6">
@@ -4493,11 +4472,11 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">30 </v>
       </c>
-      <c r="I15" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="21">
+      <c r="I15" s="7">
+        <f t="shared" si="2"/>
+        <v>1.6025806451612903</v>
+      </c>
+      <c r="J15" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4527,7 +4506,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4560,7 +4539,7 @@
         <f t="shared" si="2"/>
         <v>1.4131702460531927</v>
       </c>
-      <c r="J17" s="21"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -4587,7 +4566,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4617,7 +4596,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4644,7 +4623,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4674,37 +4653,37 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23">
-        <v>10</v>
-      </c>
-      <c r="F22" s="24">
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22">
+        <v>10</v>
+      </c>
+      <c r="F22" s="23">
         <v>1.6240000000000001</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="23">
         <f>F22*$L$2</f>
         <v>4.0648720000000003</v>
       </c>
-      <c r="H22" s="23" t="str">
+      <c r="H22" s="22" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">38 </v>
       </c>
-      <c r="I22" s="24" t="e">
+      <c r="I22" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4715,172 +4694,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B68F9BF-3EDD-47CF-B722-68B16E780082}">
-  <dimension ref="A1:N19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="M2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="L3">
-        <v>1.875</v>
-      </c>
-      <c r="M3" s="16">
-        <v>5.62</v>
-      </c>
-      <c r="N3">
-        <f>M3*10</f>
-        <v>56.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="C8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>